<commit_message>
Added max-order + sparse grids
</commit_message>
<xml_diff>
--- a/sims/code/dg-int/Vlasov-Cost-Scaling.xlsx
+++ b/sims/code/dg-int/Vlasov-Cost-Scaling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
   <si>
     <t>Vlasov Cost Scaling</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Theory Relative Cost to 1x1v</t>
+  </si>
+  <si>
+    <t>MaxOrder</t>
   </si>
 </sst>
 </file>
@@ -223,8 +226,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -331,7 +362,7 @@
     <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="117">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -376,6 +407,20 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -420,6 +465,20 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -751,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V73"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:L14"/>
+    <sheetView showRuler="0" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2208,10 +2267,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AB13"/>
+  <dimension ref="A4:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="M5" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2219,7 +2278,7 @@
     <col min="16" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:28" ht="28">
@@ -2352,7 +2411,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" ref="F9:F13" si="0">E9+D9</f>
+        <f>E9+D9</f>
         <v>3</v>
       </c>
       <c r="G9" s="7">
@@ -2369,7 +2428,7 @@
       </c>
       <c r="Q9" s="13"/>
       <c r="R9" s="13">
-        <f t="shared" ref="R9:R13" si="1">P9*G9</f>
+        <f t="shared" ref="R9:R25" si="0">P9*G9</f>
         <v>2.3152600000000003E-6</v>
       </c>
       <c r="T9" s="13">
@@ -2377,7 +2436,7 @@
         <v>2.9651921689808369</v>
       </c>
       <c r="X9" s="6">
-        <f t="shared" ref="X9:X13" si="2">(G9*I9+D9*(2*G9*I9+I9)) + (G9*M9+E9*(2*G9*M9+M9))</f>
+        <f>(G9*I9+D9*(2*G9*I9+I9)) + (G9*M9+E9*(2*G9*M9+M9))</f>
         <v>5319</v>
       </c>
       <c r="AB9" s="6">
@@ -2396,7 +2455,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" si="0"/>
+        <f>E10+D10</f>
         <v>4</v>
       </c>
       <c r="G10" s="7">
@@ -2412,7 +2471,7 @@
         <v>2.9206199999999999E-7</v>
       </c>
       <c r="R10" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4018976E-5</v>
       </c>
       <c r="T10" s="13">
@@ -2420,7 +2479,7 @@
         <v>17.95433681415059</v>
       </c>
       <c r="X10" s="6">
-        <f t="shared" si="2"/>
+        <f>(G10*I10+D10*(2*G10*I10+I10)) + (G10*M10+E10*(2*G10*M10+M10))</f>
         <v>48357</v>
       </c>
       <c r="AB10" s="6">
@@ -2439,7 +2498,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" si="0"/>
+        <f>E11+D11</f>
         <v>4</v>
       </c>
       <c r="G11" s="7">
@@ -2455,7 +2514,7 @@
         <v>3.3013099999999998E-7</v>
       </c>
       <c r="R11" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5846287999999998E-5</v>
       </c>
       <c r="T11" s="13">
@@ -2463,7 +2522,7 @@
         <v>20.294605826133996</v>
       </c>
       <c r="X11" s="6">
-        <f t="shared" si="2"/>
+        <f>(G11*I11+D11*(2*G11*I11+I11)) + (G11*M11+E11*(2*G11*M11+M11))</f>
         <v>54450</v>
       </c>
       <c r="AB11" s="6">
@@ -2482,7 +2541,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="0"/>
+        <f>E12+D12</f>
         <v>5</v>
       </c>
       <c r="G12" s="7">
@@ -2498,7 +2557,7 @@
         <v>1.22527E-6</v>
       </c>
       <c r="R12" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.3723024E-4</v>
       </c>
       <c r="T12" s="13">
@@ -2506,7 +2565,7 @@
         <v>175.75306142522254</v>
       </c>
       <c r="X12" s="6">
-        <f t="shared" si="2"/>
+        <f>(G12*I12+D12*(2*G12*I12+I12)) + (G12*M12+E12*(2*G12*M12+M12))</f>
         <v>476550</v>
       </c>
       <c r="AB12" s="6">
@@ -2525,7 +2584,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="0"/>
+        <f>E13+D13</f>
         <v>6</v>
       </c>
       <c r="G13" s="7">
@@ -2541,7 +2600,7 @@
         <v>8.6828999999999995E-6</v>
       </c>
       <c r="R13" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.2228223999999999E-3</v>
       </c>
       <c r="T13" s="13">
@@ -2549,12 +2608,355 @@
         <v>2846.8057900690151</v>
       </c>
       <c r="X13" s="6">
-        <f t="shared" si="2"/>
+        <f>(G13*I13+D13*(2*G13*I13+I13)) + (G13*M13+E13*(2*G13*M13+M13))</f>
         <v>4410315</v>
       </c>
       <c r="AB13" s="6">
         <f>X13/X8</f>
         <v>8400.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="23">
+      <c r="F14" s="6"/>
+      <c r="R14" s="13"/>
+      <c r="X14" s="6"/>
+    </row>
+    <row r="15" spans="1:28" ht="23">
+      <c r="F15" s="6"/>
+      <c r="R15" s="13"/>
+      <c r="X15" s="6"/>
+    </row>
+    <row r="16" spans="1:28" ht="23">
+      <c r="F16" s="6"/>
+      <c r="R16" s="13"/>
+      <c r="X16" s="6"/>
+    </row>
+    <row r="17" spans="1:28" ht="23">
+      <c r="F17" s="6"/>
+      <c r="R17" s="13"/>
+      <c r="X17" s="6"/>
+    </row>
+    <row r="18" spans="1:28" ht="28">
+      <c r="A18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" s="11"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S18" s="12"/>
+      <c r="T18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="X18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y18" s="8"/>
+      <c r="AB18" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="25">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="R19" s="13"/>
+      <c r="X19" s="6"/>
+    </row>
+    <row r="20" spans="1:28" ht="23">
+      <c r="A20" s="6">
+        <v>2</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" ref="F14:F25" si="1">E20+D20</f>
+        <v>2</v>
+      </c>
+      <c r="G20" s="7">
+        <v>6</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7">
+        <v>9</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7">
+        <v>9</v>
+      </c>
+      <c r="P20" s="13">
+        <v>1.26383E-7</v>
+      </c>
+      <c r="R20" s="13">
+        <f t="shared" si="0"/>
+        <v>7.5829799999999995E-7</v>
+      </c>
+      <c r="T20" s="6">
+        <v>1</v>
+      </c>
+      <c r="X20" s="6">
+        <f t="shared" ref="X14:X25" si="2">(G20*I20+D20*(2*G20*I20+I20)) + (G20*M20+E20*(2*G20*M20+M20))</f>
+        <v>342</v>
+      </c>
+      <c r="AB20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="23">
+      <c r="A21" s="6">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
+        <v>2</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G21" s="7">
+        <v>10</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7">
+        <v>19</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7">
+        <v>19</v>
+      </c>
+      <c r="P21" s="13">
+        <v>1.3792799999999999E-7</v>
+      </c>
+      <c r="R21" s="13">
+        <f t="shared" si="0"/>
+        <v>1.3792799999999999E-6</v>
+      </c>
+      <c r="T21" s="13">
+        <f>R21/R20</f>
+        <v>1.8189155187010912</v>
+      </c>
+      <c r="X21" s="6">
+        <f t="shared" si="2"/>
+        <v>1577</v>
+      </c>
+      <c r="AB21" s="6">
+        <f>X21/X20</f>
+        <v>4.6111111111111107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" ht="23">
+      <c r="A22" s="6">
+        <v>2</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6">
+        <v>3</v>
+      </c>
+      <c r="F22" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G22" s="7">
+        <v>15</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7">
+        <v>33</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7">
+        <v>33</v>
+      </c>
+      <c r="P22" s="13">
+        <v>1.8886299999999999E-7</v>
+      </c>
+      <c r="R22" s="13">
+        <f t="shared" si="0"/>
+        <v>2.8329449999999998E-6</v>
+      </c>
+      <c r="T22" s="13">
+        <f>R22/R20</f>
+        <v>3.7359257178576231</v>
+      </c>
+      <c r="X22" s="6">
+        <f t="shared" si="2"/>
+        <v>5082</v>
+      </c>
+      <c r="AB22" s="6">
+        <f>X22/X20</f>
+        <v>14.859649122807017</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" ht="23">
+      <c r="A23" s="6">
+        <v>2</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2</v>
+      </c>
+      <c r="E23" s="7">
+        <v>2</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G23" s="7">
+        <v>15</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7">
+        <v>33</v>
+      </c>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7">
+        <v>33</v>
+      </c>
+      <c r="P23" s="13">
+        <v>1.8886299999999999E-7</v>
+      </c>
+      <c r="R23" s="13">
+        <f t="shared" si="0"/>
+        <v>2.8329449999999998E-6</v>
+      </c>
+      <c r="T23" s="13">
+        <f>R23/R20</f>
+        <v>3.7359257178576231</v>
+      </c>
+      <c r="X23" s="6">
+        <f t="shared" si="2"/>
+        <v>5082</v>
+      </c>
+      <c r="AB23" s="6">
+        <f>X23/X20</f>
+        <v>14.859649122807017</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="23">
+      <c r="A24" s="6">
+        <v>2</v>
+      </c>
+      <c r="D24" s="7">
+        <v>2</v>
+      </c>
+      <c r="E24" s="7">
+        <v>3</v>
+      </c>
+      <c r="F24" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="7">
+        <v>21</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7">
+        <v>51</v>
+      </c>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7">
+        <v>51</v>
+      </c>
+      <c r="P24" s="13">
+        <v>2.6855200000000001E-7</v>
+      </c>
+      <c r="R24" s="13">
+        <f t="shared" si="0"/>
+        <v>5.639592E-6</v>
+      </c>
+      <c r="T24" s="13">
+        <f>R24/R20</f>
+        <v>7.4371711385233779</v>
+      </c>
+      <c r="X24" s="6">
+        <f t="shared" si="2"/>
+        <v>13107</v>
+      </c>
+      <c r="AB24" s="6">
+        <f>X24/X20</f>
+        <v>38.324561403508774</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" ht="23">
+      <c r="A25" s="6">
+        <v>2</v>
+      </c>
+      <c r="D25" s="7">
+        <v>3</v>
+      </c>
+      <c r="E25" s="7">
+        <v>3</v>
+      </c>
+      <c r="F25" s="6">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G25" s="7">
+        <v>28</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7">
+        <v>73</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7">
+        <v>73</v>
+      </c>
+      <c r="P25" s="13">
+        <v>3.4489299999999999E-7</v>
+      </c>
+      <c r="R25" s="13">
+        <f t="shared" si="0"/>
+        <v>9.6570040000000001E-6</v>
+      </c>
+      <c r="T25" s="13">
+        <f>R25/R20</f>
+        <v>12.735104141116027</v>
+      </c>
+      <c r="X25" s="6">
+        <f t="shared" si="2"/>
+        <v>29054</v>
+      </c>
+      <c r="AB25" s="6">
+        <f>X25/X20</f>
+        <v>84.953216374269005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with max-order basis data
</commit_message>
<xml_diff>
--- a/sims/code/dg-int/Vlasov-Cost-Scaling.xlsx
+++ b/sims/code/dg-int/Vlasov-Cost-Scaling.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="27">
   <si>
     <t>Vlasov Cost Scaling</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>MaxOrder</t>
+  </si>
+  <si>
+    <t>Relative Cost to Serendipity</t>
   </si>
 </sst>
 </file>
@@ -226,8 +229,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="117">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -362,7 +369,7 @@
     <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="117">
+  <cellStyles count="121">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -421,6 +428,8 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -479,6 +488,8 @@
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2267,10 +2278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AB25"/>
+  <dimension ref="A4:AG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="M5" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="Q7" workbookViewId="0">
+      <selection activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2279,6 +2290,7 @@
     <col min="17" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:28" ht="28">
@@ -2368,7 +2380,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="6">
-        <f>E8+D8</f>
+        <f t="shared" ref="F8:F13" si="0">E8+D8</f>
         <v>2</v>
       </c>
       <c r="G8" s="7">
@@ -2393,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="X8" s="6">
-        <f>(G8*I8+D8*(2*G8*I8+I8)) + (G8*M8+E8*(2*G8*M8+M8))</f>
+        <f t="shared" ref="X8:X13" si="1">(G8*I8+D8*(2*G8*I8+I8)) + (G8*M8+E8*(2*G8*M8+M8))</f>
         <v>525</v>
       </c>
       <c r="AB8" s="6">
@@ -2411,7 +2423,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="6">
-        <f>E9+D9</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G9" s="7">
@@ -2428,7 +2440,7 @@
       </c>
       <c r="Q9" s="13"/>
       <c r="R9" s="13">
-        <f t="shared" ref="R9:R25" si="0">P9*G9</f>
+        <f t="shared" ref="R9:R25" si="2">P9*G9</f>
         <v>2.3152600000000003E-6</v>
       </c>
       <c r="T9" s="13">
@@ -2436,7 +2448,7 @@
         <v>2.9651921689808369</v>
       </c>
       <c r="X9" s="6">
-        <f>(G9*I9+D9*(2*G9*I9+I9)) + (G9*M9+E9*(2*G9*M9+M9))</f>
+        <f t="shared" si="1"/>
         <v>5319</v>
       </c>
       <c r="AB9" s="6">
@@ -2455,7 +2467,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="6">
-        <f>E10+D10</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G10" s="7">
@@ -2471,7 +2483,7 @@
         <v>2.9206199999999999E-7</v>
       </c>
       <c r="R10" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.4018976E-5</v>
       </c>
       <c r="T10" s="13">
@@ -2479,7 +2491,7 @@
         <v>17.95433681415059</v>
       </c>
       <c r="X10" s="6">
-        <f>(G10*I10+D10*(2*G10*I10+I10)) + (G10*M10+E10*(2*G10*M10+M10))</f>
+        <f t="shared" si="1"/>
         <v>48357</v>
       </c>
       <c r="AB10" s="6">
@@ -2498,7 +2510,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="6">
-        <f>E11+D11</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G11" s="7">
@@ -2514,7 +2526,7 @@
         <v>3.3013099999999998E-7</v>
       </c>
       <c r="R11" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.5846287999999998E-5</v>
       </c>
       <c r="T11" s="13">
@@ -2522,7 +2534,7 @@
         <v>20.294605826133996</v>
       </c>
       <c r="X11" s="6">
-        <f>(G11*I11+D11*(2*G11*I11+I11)) + (G11*M11+E11*(2*G11*M11+M11))</f>
+        <f t="shared" si="1"/>
         <v>54450</v>
       </c>
       <c r="AB11" s="6">
@@ -2541,7 +2553,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="6">
-        <f>E12+D12</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G12" s="7">
@@ -2557,7 +2569,7 @@
         <v>1.22527E-6</v>
       </c>
       <c r="R12" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.3723024E-4</v>
       </c>
       <c r="T12" s="13">
@@ -2565,7 +2577,7 @@
         <v>175.75306142522254</v>
       </c>
       <c r="X12" s="6">
-        <f>(G12*I12+D12*(2*G12*I12+I12)) + (G12*M12+E12*(2*G12*M12+M12))</f>
+        <f t="shared" si="1"/>
         <v>476550</v>
       </c>
       <c r="AB12" s="6">
@@ -2584,7 +2596,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="6">
-        <f>E13+D13</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G13" s="7">
@@ -2600,7 +2612,7 @@
         <v>8.6828999999999995E-6</v>
       </c>
       <c r="R13" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.2228223999999999E-3</v>
       </c>
       <c r="T13" s="13">
@@ -2608,7 +2620,7 @@
         <v>2846.8057900690151</v>
       </c>
       <c r="X13" s="6">
-        <f>(G13*I13+D13*(2*G13*I13+I13)) + (G13*M13+E13*(2*G13*M13+M13))</f>
+        <f t="shared" si="1"/>
         <v>4410315</v>
       </c>
       <c r="AB13" s="6">
@@ -2631,12 +2643,12 @@
       <c r="R16" s="13"/>
       <c r="X16" s="6"/>
     </row>
-    <row r="17" spans="1:28" ht="23">
+    <row r="17" spans="1:33" ht="23">
       <c r="F17" s="6"/>
       <c r="R17" s="13"/>
       <c r="X17" s="6"/>
     </row>
-    <row r="18" spans="1:28" ht="28">
+    <row r="18" spans="1:33" ht="28">
       <c r="A18" s="8" t="s">
         <v>1</v>
       </c>
@@ -2682,8 +2694,11 @@
       <c r="AB18" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" ht="25">
+      <c r="AG18" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" ht="25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -2691,7 +2706,7 @@
       <c r="R19" s="13"/>
       <c r="X19" s="6"/>
     </row>
-    <row r="20" spans="1:28" ht="23">
+    <row r="20" spans="1:33" ht="23">
       <c r="A20" s="6">
         <v>2</v>
       </c>
@@ -2702,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="6">
-        <f t="shared" ref="F14:F25" si="1">E20+D20</f>
+        <f t="shared" ref="F20:F25" si="3">E20+D20</f>
         <v>2</v>
       </c>
       <c r="G20" s="7">
@@ -2720,21 +2735,25 @@
         <v>1.26383E-7</v>
       </c>
       <c r="R20" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7.5829799999999995E-7</v>
       </c>
       <c r="T20" s="6">
         <v>1</v>
       </c>
       <c r="X20" s="6">
-        <f t="shared" ref="X14:X25" si="2">(G20*I20+D20*(2*G20*I20+I20)) + (G20*M20+E20*(2*G20*M20+M20))</f>
+        <f t="shared" ref="X20:X25" si="4">(G20*I20+D20*(2*G20*I20+I20)) + (G20*M20+E20*(2*G20*M20+M20))</f>
         <v>342</v>
       </c>
       <c r="AB20" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" ht="23">
+      <c r="AG20" s="13">
+        <f>R8/R20</f>
+        <v>1.0296912295693776</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" ht="23">
       <c r="A21" s="6">
         <v>2</v>
       </c>
@@ -2745,7 +2764,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="G21" s="7">
@@ -2763,7 +2782,7 @@
         <v>1.3792799999999999E-7</v>
       </c>
       <c r="R21" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.3792799999999999E-6</v>
       </c>
       <c r="T21" s="13">
@@ -2771,15 +2790,19 @@
         <v>1.8189155187010912</v>
       </c>
       <c r="X21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1577</v>
       </c>
       <c r="AB21" s="6">
         <f>X21/X20</f>
         <v>4.6111111111111107</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" ht="23">
+      <c r="AG21" s="13">
+        <f t="shared" ref="AG21:AG25" si="5">R9/R21</f>
+        <v>1.678600429209443</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" ht="23">
       <c r="A22" s="6">
         <v>2</v>
       </c>
@@ -2790,7 +2813,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G22" s="7">
@@ -2808,7 +2831,7 @@
         <v>1.8886299999999999E-7</v>
       </c>
       <c r="R22" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.8329449999999998E-6</v>
       </c>
       <c r="T22" s="13">
@@ -2816,15 +2839,19 @@
         <v>3.7359257178576231</v>
       </c>
       <c r="X22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5082</v>
       </c>
       <c r="AB22" s="6">
         <f>X22/X20</f>
         <v>14.859649122807017</v>
       </c>
-    </row>
-    <row r="23" spans="1:28" ht="23">
+      <c r="AG22" s="13">
+        <f t="shared" si="5"/>
+        <v>4.9485521250853797</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" ht="23">
       <c r="A23" s="6">
         <v>2</v>
       </c>
@@ -2835,7 +2862,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G23" s="7">
@@ -2853,7 +2880,7 @@
         <v>1.8886299999999999E-7</v>
       </c>
       <c r="R23" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.8329449999999998E-6</v>
       </c>
       <c r="T23" s="13">
@@ -2861,15 +2888,19 @@
         <v>3.7359257178576231</v>
       </c>
       <c r="X23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5082</v>
       </c>
       <c r="AB23" s="6">
         <f>X23/X20</f>
         <v>14.859649122807017</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" ht="23">
+      <c r="AG23" s="13">
+        <f t="shared" si="5"/>
+        <v>5.5935741781079402</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" ht="23">
       <c r="A24" s="6">
         <v>2</v>
       </c>
@@ -2880,7 +2911,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G24" s="7">
@@ -2898,7 +2929,7 @@
         <v>2.6855200000000001E-7</v>
       </c>
       <c r="R24" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.639592E-6</v>
       </c>
       <c r="T24" s="13">
@@ -2906,15 +2937,19 @@
         <v>7.4371711385233779</v>
       </c>
       <c r="X24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13107</v>
       </c>
       <c r="AB24" s="6">
         <f>X24/X20</f>
         <v>38.324561403508774</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" ht="23">
+      <c r="AG24" s="13">
+        <f t="shared" si="5"/>
+        <v>24.333363122722353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" ht="23">
       <c r="A25" s="6">
         <v>2</v>
       </c>
@@ -2925,7 +2960,7 @@
         <v>3</v>
       </c>
       <c r="F25" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="G25" s="7">
@@ -2943,7 +2978,7 @@
         <v>3.4489299999999999E-7</v>
       </c>
       <c r="R25" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.6570040000000001E-6</v>
       </c>
       <c r="T25" s="13">
@@ -2951,12 +2986,16 @@
         <v>12.735104141116027</v>
       </c>
       <c r="X25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>29054</v>
       </c>
       <c r="AB25" s="6">
         <f>X25/X20</f>
         <v>84.953216374269005</v>
+      </c>
+      <c r="AG25" s="13">
+        <f t="shared" si="5"/>
+        <v>230.1772268086458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>